<commit_message>
Update project schedule (by Maysoon Magdy)
</commit_message>
<xml_diff>
--- a/TAWA_PeerReviewSheet.xlsx
+++ b/TAWA_PeerReviewSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\TAWA\Travel-Adviser-Web-Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -327,17 +327,8 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -366,6 +357,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -652,14 +652,14 @@
   <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="1.21875" customWidth="1"/>
     <col min="5" max="5" width="48.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
@@ -672,400 +672,400 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
     </row>
     <row r="2" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="6" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6" t="s">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6" t="s">
+      <c r="T2" s="3"/>
+      <c r="U2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
     </row>
     <row r="3" spans="1:25" ht="135.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="7">
         <v>43470</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
     </row>
     <row r="4" spans="1:25" ht="172.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <v>43470</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
     </row>
     <row r="5" spans="1:25" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="14" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>43470</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
     </row>
     <row r="6" spans="1:25" ht="156.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="14" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>43470</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
     </row>
     <row r="7" spans="1:25" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>43501</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
     </row>
     <row r="8" spans="1:25" ht="141" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="14" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
     </row>
     <row r="9" spans="1:25" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
-      <c r="X9" s="12"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
     </row>
     <row r="10" spans="1:25" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="14" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
the comments on the ProjectSchedule have been modified in the 'TAWA_PeerReviewSheet'document
</commit_message>
<xml_diff>
--- a/TAWA_PeerReviewSheet.xlsx
+++ b/TAWA_PeerReviewSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\TAWA\Travel-Adviser-Web-Application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\project management\project\Travel-Adviser-Web-Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -95,16 +95,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1- Review the start dates and finish dates with team members.
-2- Rename the section of work to work hours.
-3- Complete percentage is incorrect.
-4- Move the question marks from the duration section.
-5- The extension of SIQ is xlsx not word.
-6- Add TAWA_SystemRequirements.xlsx and TAWA_CustomerRequirements.xlsx
-7- The PDF version is not clear.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">1- Edit section 2.1: change “GitHub tool” to “GitHub Desktop tool”.
 2- Edit section 2.2: change “development team” to “delivery team”.
 3- Mention the documents branch in section 2.2 .
@@ -145,14 +135,24 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Accpted</t>
-  </si>
-  <si>
     <t>29/4/2019</t>
   </si>
   <si>
     <t>1,2,3 Accepted and
 4 Rejected</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Review the start dates and finish dates with the  team members.
+2- Rename the section of 'work' to 'work hours'.
+3- The Completed percentage section calculations is incorrect.
+4- Move the question marks displayed after the number of days from the 'duration' section.
+5- The extension of 'TAWA_SIQ 'document is '.xlsx 'not '.docx'.
+6- Add the' TAWA_SystemRequirements.xlsx' document and 'TAWA_CustomerRequirements.xlsx' document to the documents section.
+7- The PDF version contents of the 'project schedule' document are overlapping .
+</t>
   </si>
 </sst>
 </file>
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,53 +712,53 @@
       <c r="C2" s="16"/>
       <c r="D2" s="1"/>
       <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
@@ -781,7 +781,7 @@
         <v>43470</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="9"/>
@@ -801,7 +801,7 @@
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
     </row>
-    <row r="4" spans="1:25" ht="172.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="250.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -813,13 +813,13 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="11" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F4" s="7">
         <v>43470</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="9"/>
@@ -851,13 +851,13 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="7">
         <v>43470</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="9"/>
@@ -889,13 +889,13 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="7">
         <v>43470</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="9"/>
@@ -927,13 +927,13 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="7">
         <v>43501</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="9"/>
@@ -965,13 +965,13 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="9"/>
@@ -1003,13 +1003,13 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="9"/>
@@ -1041,13 +1041,13 @@
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="9"/>

</xml_diff>